<commit_message>
add common tool file
</commit_message>
<xml_diff>
--- a/doc/thor project.xlsx
+++ b/doc/thor project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="功能列表" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
   <si>
     <t>暂不支持</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -478,6 +478,42 @@
   </si>
   <si>
     <t>支持函数（日期函数, 字符串函数）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMPORT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 (方便测试性能）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3（最大化性能测试）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2（最大化性能测试）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4（最大化性能测试）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 方便测试其他语句</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 方便测试其他语句</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进程，工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 便于测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1264,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C41"/>
+  <dimension ref="A2:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1362,7 +1398,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -1370,7 +1406,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>93</v>
       </c>
@@ -1378,8 +1414,11 @@
       <c r="C20" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>93</v>
       </c>
@@ -1387,8 +1426,11 @@
       <c r="C21" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>93</v>
       </c>
@@ -1396,8 +1438,11 @@
       <c r="C22" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1405,7 +1450,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>93</v>
       </c>
@@ -1414,7 +1459,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>93</v>
       </c>
@@ -1422,8 +1467,11 @@
       <c r="C27" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -1431,7 +1479,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>93</v>
       </c>
@@ -1439,8 +1487,11 @@
       <c r="C31" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -1448,7 +1499,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -1456,7 +1507,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -1464,7 +1515,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>92</v>
       </c>
@@ -1473,7 +1524,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>92</v>
       </c>
@@ -1481,7 +1532,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -1489,16 +1540,45 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>90</v>
       </c>
       <c r="C41" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add thread executor base
</commit_message>
<xml_diff>
--- a/doc/thor project.xlsx
+++ b/doc/thor project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="feature &amp; function" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="172">
   <si>
     <t>暂不支持</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -674,6 +674,34 @@
   </si>
   <si>
     <t>完成了基本的导入功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liblfds-6.1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FREE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>免锁数据结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>theron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>并发操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mintomic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>？？？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1485,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
@@ -1806,11 +1834,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1933,6 +1961,15 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
       <c r="E7" t="s">
         <v>141</v>
       </c>
@@ -1994,6 +2031,25 @@
       </c>
       <c r="G14" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E15" t="s">
+        <v>168</v>
+      </c>
+      <c r="G15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E16" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>